<commit_message>
Included GVA eval excels
</commit_message>
<xml_diff>
--- a/1_Result_Tables/4_ifo_QoQ_GVA_matched_to_ifoCAST/ifo_qoq_matched_error_tables_latest_GVA.xlsx
+++ b/1_Result_Tables/4_ifo_QoQ_GVA_matched_to_ifoCAST/ifo_qoq_matched_error_tables_latest_GVA.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/1_Result_Tables/4_ifo_QoQ_GVA_matched_to_ifoCAST/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_A82AA0178421185BEC1003D0EEF2D3C26457B664" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="16950" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GVA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -67,8 +86,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,17 +146,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +202,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,9 +271,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,14 +447,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -453,33 +484,33 @@
         <v>-0.1928197451935269</v>
       </c>
       <c r="C2">
-        <v>0.7213461695319103</v>
+        <v>0.72134616953191033</v>
       </c>
       <c r="D2">
-        <v>0.8794852631762495</v>
+        <v>0.87948526317624953</v>
       </c>
       <c r="E2">
-        <v>0.937808756184463</v>
+        <v>0.93780875618446302</v>
       </c>
       <c r="F2">
-        <v>0.9393697937820958</v>
+        <v>0.93936979378209584</v>
       </c>
       <c r="G2">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.6362797032769983</v>
+        <v>0.63627970327699834</v>
       </c>
       <c r="C3">
-        <v>0.97566265080416</v>
+        <v>0.97566265080416004</v>
       </c>
       <c r="D3">
-        <v>2.153117470196778</v>
+        <v>2.1531174701967779</v>
       </c>
       <c r="E3">
         <v>1.467350493303075</v>
@@ -491,30 +522,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.4962174524051131</v>
+        <v>0.49621745240511311</v>
       </c>
       <c r="C4">
-        <v>1.236794399787266</v>
+        <v>1.2367943997872659</v>
       </c>
       <c r="D4">
-        <v>3.584317494424144</v>
+        <v>3.5843174944241438</v>
       </c>
       <c r="E4">
         <v>1.893229382410949</v>
       </c>
       <c r="F4">
-        <v>1.874506456967645</v>
+        <v>1.8745064569676451</v>
       </c>
       <c r="G4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -522,36 +553,36 @@
         <v>0.6274471299089398</v>
       </c>
       <c r="C5">
-        <v>0.8590114912114978</v>
+        <v>0.85901149121149778</v>
       </c>
       <c r="D5">
-        <v>1.063090383934936</v>
+        <v>1.0630903839349359</v>
       </c>
       <c r="E5">
         <v>1.031062744906893</v>
       </c>
       <c r="F5">
-        <v>0.8405887215707626</v>
+        <v>0.84058872157076259</v>
       </c>
       <c r="G5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.4764783664069489</v>
+        <v>0.47647836640694891</v>
       </c>
       <c r="C6">
-        <v>0.7216008406060559</v>
+        <v>0.72160084060605589</v>
       </c>
       <c r="D6">
-        <v>0.7797800353013986</v>
+        <v>0.77978003530139861</v>
       </c>
       <c r="E6">
-        <v>0.8830515473636851</v>
+        <v>0.88305154736368507</v>
       </c>
       <c r="F6">
         <v>0.7650248450273921</v>
@@ -560,99 +591,99 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.2873869318222217</v>
+        <v>0.28738693182222169</v>
       </c>
       <c r="C7">
-        <v>0.5975080706102159</v>
+        <v>0.59750807061021594</v>
       </c>
       <c r="D7">
         <v>0.491823123763305</v>
       </c>
       <c r="E7">
-        <v>0.7013010222174961</v>
+        <v>0.70130102221749613</v>
       </c>
       <c r="F7">
-        <v>0.6594003847283791</v>
+        <v>0.65940038472837914</v>
       </c>
       <c r="G7">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.2799918425184295</v>
+        <v>0.27999184251842951</v>
       </c>
       <c r="C8">
         <v>0.5332441896086979</v>
       </c>
       <c r="D8">
-        <v>0.3846468616045396</v>
+        <v>0.38464686160453959</v>
       </c>
       <c r="E8">
-        <v>0.6201990499868084</v>
+        <v>0.62019904998680842</v>
       </c>
       <c r="F8">
-        <v>0.5715489407824318</v>
+        <v>0.57154894078243179</v>
       </c>
       <c r="G8">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.3070494792929577</v>
+        <v>0.30704947929295773</v>
       </c>
       <c r="C9">
-        <v>0.4624148439892812</v>
+        <v>0.46241484398928118</v>
       </c>
       <c r="D9">
-        <v>0.2792157281860894</v>
+        <v>0.27921572818608942</v>
       </c>
       <c r="E9">
-        <v>0.5284086753508968</v>
+        <v>0.52840867535089675</v>
       </c>
       <c r="F9">
-        <v>0.4510321274556993</v>
+        <v>0.45103212745569932</v>
       </c>
       <c r="G9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.1453491486406396</v>
+        <v>0.14534914864063961</v>
       </c>
       <c r="C10">
-        <v>0.424223387566586</v>
+        <v>0.42422338756658601</v>
       </c>
       <c r="D10">
         <v>0.2511888041601692</v>
       </c>
       <c r="E10">
-        <v>0.5011873942550523</v>
+        <v>0.50118739425505232</v>
       </c>
       <c r="F10">
-        <v>0.5254283157382486</v>
+        <v>0.52542831573824855</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -660,16 +691,16 @@
         <v>0.1039188275049879</v>
       </c>
       <c r="C11">
-        <v>0.570841539690854</v>
+        <v>0.57084153969085405</v>
       </c>
       <c r="D11">
-        <v>0.3583211700553082</v>
+        <v>0.35832117005530822</v>
       </c>
       <c r="E11">
-        <v>0.5985993401727973</v>
+        <v>0.59859934017279726</v>
       </c>
       <c r="F11">
-        <v>0.7219993566603403</v>
+        <v>0.72199935666034032</v>
       </c>
       <c r="G11">
         <v>3</v>

</xml_diff>